<commit_message>
MultiLegalPile: Added information which models need to be run with Lextreme tasks and which need to be run with LexGlue tasks
</commit_message>
<xml_diff>
--- a/utils/joels_models_revision_infos_MultiLegalPile.xlsx
+++ b/utils/joels_models_revision_infos_MultiLegalPile.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vetonmatoshi/Documents/Git/LEXTREME/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660A1369-B266-FE41-9CE7-E9F7C2BC47C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6158E296-D09C-6140-A8B3-332665BB3026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="36220" windowHeight="19760" xr2:uid="{AD825961-A8D7-584B-BDDC-5CD63DE769EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35720" windowHeight="19900" xr2:uid="{AD825961-A8D7-584B-BDDC-5CD63DE769EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$C$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>_name_or_path</t>
   </si>
@@ -164,9 +164,6 @@
     <t>61727ddd0405643aeb102dbabc00cb6b0ba18df5</t>
   </si>
   <si>
-    <t>need_to_be_run</t>
-  </si>
-  <si>
     <t>main</t>
   </si>
   <si>
@@ -177,6 +174,12 @@
   </si>
   <si>
     <t>c4ede6b7b73ba882dc5d0c90d804ea967e5199f2</t>
+  </si>
+  <si>
+    <t>need_to_be_run_with_LEXTREME</t>
+  </si>
+  <si>
+    <t>need_to_be_run_with_LexGlue</t>
   </si>
 </sst>
 </file>
@@ -559,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD9E512-EFBF-A848-8A97-90FA3395400E}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,291 +574,497 @@
     <col min="2" max="2" width="52.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>3</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C35" xr:uid="{2CD9E512-EFBF-A848-8A97-90FA3395400E}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added joelito/legal-xlm-longformer-base to the list of models to be run for the mulit legal pile paper
</commit_message>
<xml_diff>
--- a/utils/joels_models_revision_infos_MultiLegalPile.xlsx
+++ b/utils/joels_models_revision_infos_MultiLegalPile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vetonmatoshi/Documents/Git/LEXTREME/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED138891-5BD6-304F-A7CA-368FF81055FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4223C18-8E8F-FC4C-A416-7FA113C0D430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{AD825961-A8D7-584B-BDDC-5CD63DE769EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{AD825961-A8D7-584B-BDDC-5CD63DE769EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
   <si>
     <t>_name_or_path</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>xlm-roberta-base</t>
+  </si>
+  <si>
+    <t>joelito/legal-xlm-longformer-base</t>
   </si>
 </sst>
 </file>
@@ -577,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD9E512-EFBF-A848-8A97-90FA3395400E}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="136" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="136" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1149,6 +1152,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D35" xr:uid="{2CD9E512-EFBF-A848-8A97-90FA3395400E}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added commit hashes for large models so that they are all at 500K steps
</commit_message>
<xml_diff>
--- a/utils/joels_models_revision_infos_MultiLegalPile.xlsx
+++ b/utils/joels_models_revision_infos_MultiLegalPile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vetonmatoshi/Documents/Git/LEXTREME/utils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelniklaus/NextCloud/PhDJoelNiklaus/Code/LEXTREME/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4223C18-8E8F-FC4C-A416-7FA113C0D430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1118058-72E2-B546-92D9-E246AE9F3E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{AD825961-A8D7-584B-BDDC-5CD63DE769EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19960" xr2:uid="{AD825961-A8D7-584B-BDDC-5CD63DE769EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>_name_or_path</t>
   </si>
@@ -198,6 +198,15 @@
   </si>
   <si>
     <t>joelito/legal-xlm-longformer-base</t>
+  </si>
+  <si>
+    <t>4238a87a6e58c2cc848bf6c66a7537f7b93c42cc</t>
+  </si>
+  <si>
+    <t>2b7fa5f583c9771f3f78dc53e5f749bff8a6b9ac</t>
+  </si>
+  <si>
+    <t>18666c053a75718c1ce78184a9dbf40c2540d002</t>
   </si>
 </sst>
 </file>
@@ -268,7 +277,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -284,7 +293,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-Design 2013–2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -572,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -582,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD9E512-EFBF-A848-8A97-90FA3395400E}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="136" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:D41"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,7 +760,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -779,7 +788,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -849,7 +858,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>

</xml_diff>